<commit_message>
started following the plan made major changes
probably going to create a secondary branch and start working from the core loop and extend outiside
</commit_message>
<xml_diff>
--- a/classes.xlsx
+++ b/classes.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="19">
   <si>
     <t>White</t>
   </si>
@@ -38,9 +38,6 @@
   </si>
   <si>
     <t>class_names</t>
-  </si>
-  <si>
-    <t>total_lessons_amount</t>
   </si>
   <si>
     <t>1A</t>
@@ -398,15 +395,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T6"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -417,24 +414,21 @@
         <v>3</v>
       </c>
       <c r="D1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" t="s">
         <v>12</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>13</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>14</v>
       </c>
-      <c r="G1" t="s">
-        <v>15</v>
-      </c>
-      <c r="T1" t="s">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>7</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
@@ -448,41 +442,62 @@
       <c r="E2">
         <v>2</v>
       </c>
-      <c r="T2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="F2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="F3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>8</v>
       </c>
-      <c r="B3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3">
-        <v>2</v>
-      </c>
-      <c r="T3">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4">
+        <v>2</v>
+      </c>
+      <c r="F4" t="s">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>9</v>
-      </c>
-      <c r="B4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4">
-        <v>2</v>
-      </c>
-      <c r="T4">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>10</v>
       </c>
       <c r="B5" t="s">
         <v>1</v>
@@ -490,13 +505,22 @@
       <c r="C5">
         <v>3</v>
       </c>
-      <c r="T5">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="D5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5">
+        <v>2</v>
+      </c>
+      <c r="F5" t="s">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B6" t="s">
         <v>2</v>
@@ -504,8 +528,17 @@
       <c r="C6">
         <v>3</v>
       </c>
-      <c r="T6">
-        <v>5</v>
+      <c r="D6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6">
+        <v>2</v>
+      </c>
+      <c r="F6" t="s">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -525,13 +558,13 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
         <v>16</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>17</v>
       </c>
       <c r="D1">
         <v>3</v>
@@ -539,13 +572,13 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" t="s">
         <v>16</v>
-      </c>
-      <c r="B2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2" t="s">
-        <v>17</v>
       </c>
       <c r="D2">
         <v>2</v>
@@ -553,13 +586,13 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" t="s">
         <v>16</v>
-      </c>
-      <c r="B3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3" t="s">
-        <v>17</v>
       </c>
       <c r="D3">
         <v>4</v>
@@ -567,13 +600,13 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B4" t="s">
         <v>0</v>
       </c>
       <c r="C4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -581,13 +614,13 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" t="s">
         <v>16</v>
-      </c>
-      <c r="B5" t="s">
-        <v>2</v>
-      </c>
-      <c r="C5" t="s">
-        <v>17</v>
       </c>
       <c r="D5">
         <v>5</v>
@@ -595,127 +628,127 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
time_table polished, minor changes
</commit_message>
<xml_diff>
--- a/classes.xlsx
+++ b/classes.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="27">
   <si>
     <t>White</t>
   </si>
@@ -95,6 +95,12 @@
   </si>
   <si>
     <t>f</t>
+  </si>
+  <si>
+    <t>g</t>
+  </si>
+  <si>
+    <t>h</t>
   </si>
 </sst>
 </file>
@@ -413,15 +419,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="280" zoomScaleNormal="280" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -444,7 +450,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -452,22 +458,28 @@
         <v>19</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="D2" t="s">
         <v>21</v>
       </c>
       <c r="E2">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="F2" t="s">
         <v>20</v>
       </c>
       <c r="G2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="H2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -475,53 +487,65 @@
         <v>19</v>
       </c>
       <c r="C3">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="D3" t="s">
         <v>21</v>
       </c>
       <c r="E3">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="F3" t="s">
         <v>20</v>
       </c>
       <c r="G3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+      <c r="H3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C4">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="D4" t="s">
         <v>23</v>
       </c>
       <c r="E4">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F4" t="s">
         <v>24</v>
       </c>
       <c r="G4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+      <c r="H4" t="s">
+        <v>26</v>
+      </c>
+      <c r="I4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C5">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="D5" t="s">
         <v>23</v>
@@ -533,18 +557,24 @@
         <v>24</v>
       </c>
       <c r="G5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+      <c r="H5" t="s">
+        <v>26</v>
+      </c>
+      <c r="I5">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C6">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="D6" t="s">
         <v>23</v>
@@ -556,7 +586,13 @@
         <v>24</v>
       </c>
       <c r="G6">
-        <v>1</v>
+        <v>7</v>
+      </c>
+      <c r="H6" t="s">
+        <v>26</v>
+      </c>
+      <c r="I6">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>